<commit_message>
Onnodige resources verwijderd, mogelijke te gebruiken lettertypes toegevoegd. MoodBoard toegevoegd, afbeeldingen van moskeen toegevoegd
</commit_message>
<xml_diff>
--- a/Documentatie/TimesheetTemplate.xlsx
+++ b/Documentatie/TimesheetTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Taak</t>
   </si>
@@ -37,6 +37,33 @@
   </si>
   <si>
     <t>Totaal</t>
+  </si>
+  <si>
+    <t>Mock up - Native APP</t>
+  </si>
+  <si>
+    <t>1h30</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>LogoComponents</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>Logo zelf</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>3h30</t>
+  </si>
+  <si>
+    <t>Moodboard</t>
   </si>
 </sst>
 </file>
@@ -156,7 +183,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -165,6 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -181,10 +209,15 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -513,17 +546,17 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD28"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" customWidth="1"/>
+    <col min="4" max="4" width="30.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -531,7 +564,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="20">
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -545,337 +578,371 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>41254</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>41262</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>41262</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>41263</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>41263</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" ht="18">
+    <row r="58" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>